<commit_message>
Optimization model functions added Frontend optimization components added
</commit_message>
<xml_diff>
--- a/OptimizationAlgorithmAPI/modified_sampledata4.xlsx
+++ b/OptimizationAlgorithmAPI/modified_sampledata4.xlsx
@@ -14544,7 +14544,7 @@
         <v>0.207583333333333</v>
       </c>
       <c r="D39" t="n">
-        <v>0.01019</v>
+        <v>0</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
@@ -14571,7 +14571,7 @@
         <v>0.390666666666667</v>
       </c>
       <c r="D40" t="n">
-        <v>0.05285</v>
+        <v>0</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
@@ -14598,7 +14598,7 @@
         <v>0.582583333333333</v>
       </c>
       <c r="D41" t="n">
-        <v>0.06597</v>
+        <v>0</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
@@ -14625,7 +14625,7 @@
         <v>1.8965</v>
       </c>
       <c r="D42" t="n">
-        <v>0.17268</v>
+        <v>0</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
@@ -14652,7 +14652,7 @@
         <v>2.33566666666667</v>
       </c>
       <c r="D43" t="n">
-        <v>0.41522</v>
+        <v>0</v>
       </c>
       <c r="E43" t="n">
         <v>0</v>
@@ -14679,7 +14679,7 @@
         <v>4.13875</v>
       </c>
       <c r="D44" t="n">
-        <v>1.06939</v>
+        <v>0</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
@@ -14706,7 +14706,7 @@
         <v>4.09875</v>
       </c>
       <c r="D45" t="n">
-        <v>1.54402</v>
+        <v>0</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
@@ -14733,7 +14733,7 @@
         <v>5.14075</v>
       </c>
       <c r="D46" t="n">
-        <v>1.22096</v>
+        <v>0</v>
       </c>
       <c r="E46" t="n">
         <v>0</v>
@@ -14760,7 +14760,7 @@
         <v>6.99333333333333</v>
       </c>
       <c r="D47" t="n">
-        <v>2.07124</v>
+        <v>0</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
@@ -14787,7 +14787,7 @@
         <v>2.64275</v>
       </c>
       <c r="D48" t="n">
-        <v>2.25089</v>
+        <v>0</v>
       </c>
       <c r="E48" t="n">
         <v>0</v>
@@ -14814,7 +14814,7 @@
         <v>7.14091666666667</v>
       </c>
       <c r="D49" t="n">
-        <v>1.93177</v>
+        <v>0</v>
       </c>
       <c r="E49" t="n">
         <v>0</v>
@@ -14841,7 +14841,7 @@
         <v>2.39025</v>
       </c>
       <c r="D50" t="n">
-        <v>1.94467</v>
+        <v>0</v>
       </c>
       <c r="E50" t="n">
         <v>0</v>
@@ -14868,7 +14868,7 @@
         <v>2.27208333333333</v>
       </c>
       <c r="D51" t="n">
-        <v>1.43851</v>
+        <v>0</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
@@ -14895,7 +14895,7 @@
         <v>5.96733333333333</v>
       </c>
       <c r="D52" t="n">
-        <v>1.21495</v>
+        <v>0</v>
       </c>
       <c r="E52" t="n">
         <v>0</v>
@@ -14922,7 +14922,7 @@
         <v>6.55975</v>
       </c>
       <c r="D53" t="n">
-        <v>1.09185</v>
+        <v>0</v>
       </c>
       <c r="E53" t="n">
         <v>0</v>
@@ -14949,7 +14949,7 @@
         <v>2.73341666666667</v>
       </c>
       <c r="D54" t="n">
-        <v>1.41578</v>
+        <v>0</v>
       </c>
       <c r="E54" t="n">
         <v>0</v>
@@ -14976,7 +14976,7 @@
         <v>5.4705</v>
       </c>
       <c r="D55" t="n">
-        <v>1.19308</v>
+        <v>0</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
@@ -15003,7 +15003,7 @@
         <v>3.90991666666667</v>
       </c>
       <c r="D56" t="n">
-        <v>0.71994</v>
+        <v>0</v>
       </c>
       <c r="E56" t="n">
         <v>0</v>
@@ -15030,7 +15030,7 @@
         <v>3.93191666666667</v>
       </c>
       <c r="D57" t="n">
-        <v>0.47953</v>
+        <v>0</v>
       </c>
       <c r="E57" t="n">
         <v>0</v>
@@ -15057,7 +15057,7 @@
         <v>4.69641666666667</v>
       </c>
       <c r="D58" t="n">
-        <v>0.5771500000000001</v>
+        <v>0</v>
       </c>
       <c r="E58" t="n">
         <v>0</v>
@@ -15084,7 +15084,7 @@
         <v>4.43475</v>
       </c>
       <c r="D59" t="n">
-        <v>0.7019300000000001</v>
+        <v>0</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
@@ -15111,7 +15111,7 @@
         <v>4.69941666666667</v>
       </c>
       <c r="D60" t="n">
-        <v>0.58473</v>
+        <v>0</v>
       </c>
       <c r="E60" t="n">
         <v>0</v>
@@ -15138,7 +15138,7 @@
         <v>4.10258333333333</v>
       </c>
       <c r="D61" t="n">
-        <v>0.67397</v>
+        <v>0</v>
       </c>
       <c r="E61" t="n">
         <v>0</v>
@@ -15165,7 +15165,7 @@
         <v>3.02808333333333</v>
       </c>
       <c r="D62" t="n">
-        <v>0.45674</v>
+        <v>0</v>
       </c>
       <c r="E62" t="n">
         <v>0</v>
@@ -15192,7 +15192,7 @@
         <v>2.13133333333333</v>
       </c>
       <c r="D63" t="n">
-        <v>0.35154</v>
+        <v>0</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
@@ -15219,7 +15219,7 @@
         <v>1.83833333333333</v>
       </c>
       <c r="D64" t="n">
-        <v>0.26225</v>
+        <v>0</v>
       </c>
       <c r="E64" t="n">
         <v>0</v>
@@ -15246,7 +15246,7 @@
         <v>1.38708333333333</v>
       </c>
       <c r="D65" t="n">
-        <v>0.22227</v>
+        <v>0</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
@@ -15273,7 +15273,7 @@
         <v>0.839833333333333</v>
       </c>
       <c r="D66" t="n">
-        <v>0.14198</v>
+        <v>0</v>
       </c>
       <c r="E66" t="n">
         <v>0</v>
@@ -15300,7 +15300,7 @@
         <v>0.827583333333333</v>
       </c>
       <c r="D67" t="n">
-        <v>0.10399</v>
+        <v>0</v>
       </c>
       <c r="E67" t="n">
         <v>0</v>
@@ -15327,7 +15327,7 @@
         <v>0.563166666666667</v>
       </c>
       <c r="D68" t="n">
-        <v>0.09693</v>
+        <v>0</v>
       </c>
       <c r="E68" t="n">
         <v>0</v>
@@ -15354,7 +15354,7 @@
         <v>0.3755</v>
       </c>
       <c r="D69" t="n">
-        <v>0.05683</v>
+        <v>0</v>
       </c>
       <c r="E69" t="n">
         <v>0</v>
@@ -15381,7 +15381,7 @@
         <v>0.208666666666667</v>
       </c>
       <c r="D70" t="n">
-        <v>0.04233</v>
+        <v>0</v>
       </c>
       <c r="E70" t="n">
         <v>0</v>
@@ -15408,7 +15408,7 @@
         <v>0.166</v>
       </c>
       <c r="D71" t="n">
-        <v>0.01289</v>
+        <v>0</v>
       </c>
       <c r="E71" t="n">
         <v>0</v>
@@ -15435,7 +15435,7 @@
         <v>0.189</v>
       </c>
       <c r="D72" t="n">
-        <v>0.02279</v>
+        <v>0</v>
       </c>
       <c r="E72" t="n">
         <v>0</v>
@@ -15462,7 +15462,7 @@
         <v>0.02425</v>
       </c>
       <c r="D73" t="n">
-        <v>0.01202</v>
+        <v>0</v>
       </c>
       <c r="E73" t="n">
         <v>0</v>
@@ -17190,7 +17190,7 @@
         <v>0.1805</v>
       </c>
       <c r="D137" t="n">
-        <v>0.0009700000000000001</v>
+        <v>0</v>
       </c>
       <c r="E137" t="n">
         <v>0</v>
@@ -17217,7 +17217,7 @@
         <v>0.25525</v>
       </c>
       <c r="D138" t="n">
-        <v>0.03133</v>
+        <v>0</v>
       </c>
       <c r="E138" t="n">
         <v>0</v>
@@ -17244,7 +17244,7 @@
         <v>0.15825</v>
       </c>
       <c r="D139" t="n">
-        <v>0.0119</v>
+        <v>0</v>
       </c>
       <c r="E139" t="n">
         <v>0</v>
@@ -17271,7 +17271,7 @@
         <v>0.376166666666667</v>
       </c>
       <c r="D140" t="n">
-        <v>0.0286</v>
+        <v>0</v>
       </c>
       <c r="E140" t="n">
         <v>0</v>
@@ -17298,7 +17298,7 @@
         <v>0.443833333333333</v>
       </c>
       <c r="D141" t="n">
-        <v>0.06393</v>
+        <v>0</v>
       </c>
       <c r="E141" t="n">
         <v>0</v>
@@ -17325,7 +17325,7 @@
         <v>0.833666666666667</v>
       </c>
       <c r="D142" t="n">
-        <v>0.05904</v>
+        <v>0</v>
       </c>
       <c r="E142" t="n">
         <v>0</v>
@@ -17352,7 +17352,7 @@
         <v>0.66925</v>
       </c>
       <c r="D143" t="n">
-        <v>0.11905</v>
+        <v>0</v>
       </c>
       <c r="E143" t="n">
         <v>0</v>
@@ -17379,7 +17379,7 @@
         <v>0.293083333333333</v>
       </c>
       <c r="D144" t="n">
-        <v>0.05035</v>
+        <v>0</v>
       </c>
       <c r="E144" t="n">
         <v>0</v>
@@ -17406,7 +17406,7 @@
         <v>0.309166666666667</v>
       </c>
       <c r="D145" t="n">
-        <v>0.0398</v>
+        <v>0</v>
       </c>
       <c r="E145" t="n">
         <v>0</v>
@@ -17433,7 +17433,7 @@
         <v>0.40775</v>
       </c>
       <c r="D146" t="n">
-        <v>0.04922</v>
+        <v>0</v>
       </c>
       <c r="E146" t="n">
         <v>0</v>
@@ -17460,7 +17460,7 @@
         <v>0.6025</v>
       </c>
       <c r="D147" t="n">
-        <v>0.05851</v>
+        <v>0</v>
       </c>
       <c r="E147" t="n">
         <v>0</v>
@@ -17487,7 +17487,7 @@
         <v>0.7989166666666671</v>
       </c>
       <c r="D148" t="n">
-        <v>0.09027</v>
+        <v>0</v>
       </c>
       <c r="E148" t="n">
         <v>0</v>
@@ -17514,7 +17514,7 @@
         <v>0.958333333333333</v>
       </c>
       <c r="D149" t="n">
-        <v>0.10469</v>
+        <v>0</v>
       </c>
       <c r="E149" t="n">
         <v>0</v>
@@ -17541,7 +17541,7 @@
         <v>0.491416666666667</v>
       </c>
       <c r="D150" t="n">
-        <v>0.11294</v>
+        <v>0</v>
       </c>
       <c r="E150" t="n">
         <v>0</v>
@@ -17568,7 +17568,7 @@
         <v>0.425083333333333</v>
       </c>
       <c r="D151" t="n">
-        <v>0.05849</v>
+        <v>0</v>
       </c>
       <c r="E151" t="n">
         <v>0</v>
@@ -17595,7 +17595,7 @@
         <v>0.249333333333333</v>
       </c>
       <c r="D152" t="n">
-        <v>0.04263</v>
+        <v>0</v>
       </c>
       <c r="E152" t="n">
         <v>0</v>
@@ -17622,7 +17622,7 @@
         <v>0.59975</v>
       </c>
       <c r="D153" t="n">
-        <v>0.04278</v>
+        <v>0</v>
       </c>
       <c r="E153" t="n">
         <v>0</v>
@@ -17649,7 +17649,7 @@
         <v>0.810166666666667</v>
       </c>
       <c r="D154" t="n">
-        <v>0.09211</v>
+        <v>0</v>
       </c>
       <c r="E154" t="n">
         <v>0</v>
@@ -17676,7 +17676,7 @@
         <v>0.6315833333333331</v>
       </c>
       <c r="D155" t="n">
-        <v>0.10823</v>
+        <v>0</v>
       </c>
       <c r="E155" t="n">
         <v>0</v>
@@ -17703,7 +17703,7 @@
         <v>0.55825</v>
       </c>
       <c r="D156" t="n">
-        <v>0.07847999999999999</v>
+        <v>0</v>
       </c>
       <c r="E156" t="n">
         <v>0</v>
@@ -17730,7 +17730,7 @@
         <v>0.506083333333333</v>
       </c>
       <c r="D157" t="n">
-        <v>0.06838</v>
+        <v>0</v>
       </c>
       <c r="E157" t="n">
         <v>0</v>
@@ -17757,7 +17757,7 @@
         <v>0.63975</v>
       </c>
       <c r="D158" t="n">
-        <v>0.06748999999999999</v>
+        <v>0</v>
       </c>
       <c r="E158" t="n">
         <v>0</v>
@@ -17784,7 +17784,7 @@
         <v>1.17308333333333</v>
       </c>
       <c r="D159" t="n">
-        <v>0.11175</v>
+        <v>0</v>
       </c>
       <c r="E159" t="n">
         <v>0</v>
@@ -17811,7 +17811,7 @@
         <v>1.014</v>
       </c>
       <c r="D160" t="n">
-        <v>0.17127</v>
+        <v>0</v>
       </c>
       <c r="E160" t="n">
         <v>0</v>
@@ -17838,7 +17838,7 @@
         <v>0.78425</v>
       </c>
       <c r="D161" t="n">
-        <v>0.11551</v>
+        <v>0</v>
       </c>
       <c r="E161" t="n">
         <v>0</v>
@@ -17865,7 +17865,7 @@
         <v>1.28408333333333</v>
       </c>
       <c r="D162" t="n">
-        <v>0.11794</v>
+        <v>0</v>
       </c>
       <c r="E162" t="n">
         <v>0</v>
@@ -17892,7 +17892,7 @@
         <v>1.15408333333333</v>
       </c>
       <c r="D163" t="n">
-        <v>0.16065</v>
+        <v>0</v>
       </c>
       <c r="E163" t="n">
         <v>0</v>
@@ -17919,7 +17919,7 @@
         <v>1.14116666666667</v>
       </c>
       <c r="D164" t="n">
-        <v>0.16257</v>
+        <v>0</v>
       </c>
       <c r="E164" t="n">
         <v>0</v>
@@ -17946,7 +17946,7 @@
         <v>0.380166666666667</v>
       </c>
       <c r="D165" t="n">
-        <v>0.09658</v>
+        <v>0</v>
       </c>
       <c r="E165" t="n">
         <v>0</v>
@@ -17973,7 +17973,7 @@
         <v>0.243083333333333</v>
       </c>
       <c r="D166" t="n">
-        <v>0.05128</v>
+        <v>0</v>
       </c>
       <c r="E166" t="n">
         <v>0</v>
@@ -18000,7 +18000,7 @@
         <v>0.205916666666667</v>
       </c>
       <c r="D167" t="n">
-        <v>0.0155</v>
+        <v>0</v>
       </c>
       <c r="E167" t="n">
         <v>0</v>
@@ -18027,7 +18027,7 @@
         <v>0.114833333333333</v>
       </c>
       <c r="D168" t="n">
-        <v>0.02459</v>
+        <v>0</v>
       </c>
       <c r="E168" t="n">
         <v>0</v>
@@ -18054,7 +18054,7 @@
         <v>0.02525</v>
       </c>
       <c r="D169" t="n">
-        <v>0.00462</v>
+        <v>0</v>
       </c>
       <c r="E169" t="n">
         <v>0</v>
@@ -19755,7 +19755,7 @@
         <v>0.349333333333333</v>
       </c>
       <c r="D232" t="n">
-        <v>0.01927</v>
+        <v>0</v>
       </c>
       <c r="E232" t="n">
         <v>0</v>
@@ -19782,7 +19782,7 @@
         <v>0.79375</v>
       </c>
       <c r="D233" t="n">
-        <v>0.07868</v>
+        <v>0</v>
       </c>
       <c r="E233" t="n">
         <v>0</v>
@@ -19809,7 +19809,7 @@
         <v>1.25458333333333</v>
       </c>
       <c r="D234" t="n">
-        <v>0.17326</v>
+        <v>0</v>
       </c>
       <c r="E234" t="n">
         <v>0</v>
@@ -19836,7 +19836,7 @@
         <v>1.60175</v>
       </c>
       <c r="D235" t="n">
-        <v>0.22827</v>
+        <v>0</v>
       </c>
       <c r="E235" t="n">
         <v>0</v>
@@ -19863,7 +19863,7 @@
         <v>1.65033333333333</v>
       </c>
       <c r="D236" t="n">
-        <v>0.2767</v>
+        <v>0</v>
       </c>
       <c r="E236" t="n">
         <v>0</v>
@@ -19890,7 +19890,7 @@
         <v>1.78191666666667</v>
       </c>
       <c r="D237" t="n">
-        <v>0.28224</v>
+        <v>0</v>
       </c>
       <c r="E237" t="n">
         <v>0</v>
@@ -19917,7 +19917,7 @@
         <v>2.82075</v>
       </c>
       <c r="D238" t="n">
-        <v>0.31968</v>
+        <v>0</v>
       </c>
       <c r="E238" t="n">
         <v>0</v>
@@ -19944,7 +19944,7 @@
         <v>3.51991666666667</v>
       </c>
       <c r="D239" t="n">
-        <v>0.50018</v>
+        <v>0</v>
       </c>
       <c r="E239" t="n">
         <v>0</v>
@@ -19971,7 +19971,7 @@
         <v>3.66875</v>
       </c>
       <c r="D240" t="n">
-        <v>0.51133</v>
+        <v>0</v>
       </c>
       <c r="E240" t="n">
         <v>0</v>
@@ -19998,7 +19998,7 @@
         <v>4.35125</v>
       </c>
       <c r="D241" t="n">
-        <v>0.5499000000000001</v>
+        <v>0</v>
       </c>
       <c r="E241" t="n">
         <v>0</v>
@@ -20025,7 +20025,7 @@
         <v>4.036</v>
       </c>
       <c r="D242" t="n">
-        <v>0.64629</v>
+        <v>0</v>
       </c>
       <c r="E242" t="n">
         <v>0</v>
@@ -20052,7 +20052,7 @@
         <v>2.54575</v>
       </c>
       <c r="D243" t="n">
-        <v>0.52093</v>
+        <v>0</v>
       </c>
       <c r="E243" t="n">
         <v>0</v>
@@ -20079,7 +20079,7 @@
         <v>1.4655</v>
       </c>
       <c r="D244" t="n">
-        <v>0.35405</v>
+        <v>0</v>
       </c>
       <c r="E244" t="n">
         <v>0</v>
@@ -20106,7 +20106,7 @@
         <v>1.23925</v>
       </c>
       <c r="D245" t="n">
-        <v>0.21664</v>
+        <v>0</v>
       </c>
       <c r="E245" t="n">
         <v>0</v>
@@ -20133,7 +20133,7 @@
         <v>2.13108333333333</v>
       </c>
       <c r="D246" t="n">
-        <v>0.24448</v>
+        <v>0</v>
       </c>
       <c r="E246" t="n">
         <v>0</v>
@@ -20160,7 +20160,7 @@
         <v>3.31583333333333</v>
       </c>
       <c r="D247" t="n">
-        <v>0.53234</v>
+        <v>0</v>
       </c>
       <c r="E247" t="n">
         <v>0</v>
@@ -20187,7 +20187,7 @@
         <v>5.29225</v>
       </c>
       <c r="D248" t="n">
-        <v>0.7569</v>
+        <v>0</v>
       </c>
       <c r="E248" t="n">
         <v>0</v>
@@ -20214,7 +20214,7 @@
         <v>6.26916666666667</v>
       </c>
       <c r="D249" t="n">
-        <v>1.12869</v>
+        <v>0</v>
       </c>
       <c r="E249" t="n">
         <v>0</v>
@@ -20241,7 +20241,7 @@
         <v>6.00766666666667</v>
       </c>
       <c r="D250" t="n">
-        <v>2.15495</v>
+        <v>0</v>
       </c>
       <c r="E250" t="n">
         <v>0</v>
@@ -20268,7 +20268,7 @@
         <v>5.73358333333333</v>
       </c>
       <c r="D251" t="n">
-        <v>1.40109</v>
+        <v>0</v>
       </c>
       <c r="E251" t="n">
         <v>0</v>
@@ -20295,7 +20295,7 @@
         <v>6.812</v>
       </c>
       <c r="D252" t="n">
-        <v>1.1436</v>
+        <v>0</v>
       </c>
       <c r="E252" t="n">
         <v>0</v>
@@ -20322,7 +20322,7 @@
         <v>3.18816666666667</v>
       </c>
       <c r="D253" t="n">
-        <v>1.96502</v>
+        <v>0</v>
       </c>
       <c r="E253" t="n">
         <v>0</v>
@@ -20349,7 +20349,7 @@
         <v>2.87366666666667</v>
       </c>
       <c r="D254" t="n">
-        <v>2.02587</v>
+        <v>0</v>
       </c>
       <c r="E254" t="n">
         <v>0</v>
@@ -20376,7 +20376,7 @@
         <v>5.06575</v>
       </c>
       <c r="D255" t="n">
-        <v>1.89353</v>
+        <v>0</v>
       </c>
       <c r="E255" t="n">
         <v>0</v>
@@ -20403,7 +20403,7 @@
         <v>3.50575</v>
       </c>
       <c r="D256" t="n">
-        <v>0.82582</v>
+        <v>0</v>
       </c>
       <c r="E256" t="n">
         <v>0</v>
@@ -20430,7 +20430,7 @@
         <v>6.69708333333333</v>
       </c>
       <c r="D257" t="n">
-        <v>1.19377</v>
+        <v>0</v>
       </c>
       <c r="E257" t="n">
         <v>0</v>
@@ -20457,7 +20457,7 @@
         <v>5.14041666666667</v>
       </c>
       <c r="D258" t="n">
-        <v>1.39551</v>
+        <v>0</v>
       </c>
       <c r="E258" t="n">
         <v>0</v>
@@ -20484,7 +20484,7 @@
         <v>3.95308333333333</v>
       </c>
       <c r="D259" t="n">
-        <v>1.28225</v>
+        <v>0</v>
       </c>
       <c r="E259" t="n">
         <v>0</v>
@@ -20511,7 +20511,7 @@
         <v>2.51216666666667</v>
       </c>
       <c r="D260" t="n">
-        <v>0.6569700000000001</v>
+        <v>0</v>
       </c>
       <c r="E260" t="n">
         <v>0</v>
@@ -20538,7 +20538,7 @@
         <v>0.72975</v>
       </c>
       <c r="D261" t="n">
-        <v>0.21747</v>
+        <v>0</v>
       </c>
       <c r="E261" t="n">
         <v>0</v>
@@ -20565,7 +20565,7 @@
         <v>1.2015</v>
       </c>
       <c r="D262" t="n">
-        <v>0.06307</v>
+        <v>0</v>
       </c>
       <c r="E262" t="n">
         <v>0</v>
@@ -20592,7 +20592,7 @@
         <v>1.27925</v>
       </c>
       <c r="D263" t="n">
-        <v>0.31409</v>
+        <v>0</v>
       </c>
       <c r="E263" t="n">
         <v>0</v>
@@ -20619,7 +20619,7 @@
         <v>0.770166666666667</v>
       </c>
       <c r="D264" t="n">
-        <v>0.23689</v>
+        <v>0</v>
       </c>
       <c r="E264" t="n">
         <v>0</v>
@@ -20646,7 +20646,7 @@
         <v>0.314166666666667</v>
       </c>
       <c r="D265" t="n">
-        <v>0.13698</v>
+        <v>0</v>
       </c>
       <c r="E265" t="n">
         <v>0</v>
@@ -20673,7 +20673,7 @@
         <v>0.0948333333333333</v>
       </c>
       <c r="D266" t="n">
-        <v>0.03518</v>
+        <v>0</v>
       </c>
       <c r="E266" t="n">
         <v>0</v>
@@ -20700,7 +20700,7 @@
         <v>0.00308333333333333</v>
       </c>
       <c r="D267" t="n">
-        <v>0.00412</v>
+        <v>0</v>
       </c>
       <c r="E267" t="n">
         <v>0</v>

</xml_diff>